<commit_message>
Domain Model Class details Stock_details_spec
Signed-off-by: chavp <my.parinya@gmail.com>
</commit_message>
<xml_diff>
--- a/DetailsSpec/Stock_details_spec.xlsx
+++ b/DetailsSpec/Stock_details_spec.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29F8F25-EAD2-43B0-A0B7-FBB95FC10D03}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1406E5CF-CDC2-4440-820E-98ABEA047D7F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>#</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Class Diagram</t>
   </si>
   <si>
-    <t>InventoriesService</t>
-  </si>
-  <si>
     <t>ShipmentPackageRepository</t>
   </si>
   <si>
@@ -95,13 +92,40 @@
   </si>
   <si>
     <t>Web Services</t>
+  </si>
+  <si>
+    <t>Packages</t>
+  </si>
+  <si>
+    <t>Sahapat.Shipments.IRepositories</t>
+  </si>
+  <si>
+    <t>Sahapat.StockService.Interfaces</t>
+  </si>
+  <si>
+    <t>Sahapat.Shipments.IServices</t>
+  </si>
+  <si>
+    <t>Sahapat.Shipments.Models</t>
+  </si>
+  <si>
+    <t>Sahapat.Products.IServices</t>
+  </si>
+  <si>
+    <t>Sahapat.Products.Models</t>
+  </si>
+  <si>
+    <t>ProductsService</t>
+  </si>
+  <si>
+    <t>Sahapat.Products.IRepositories</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,16 +141,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -134,14 +172,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -423,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,26 +485,30 @@
     <col min="3" max="3" width="61.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -465,122 +518,167 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+      <c r="F11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
         <v>13</v>
       </c>
-      <c r="E13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>14</v>
       </c>
-      <c r="E14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="G1GN3B11D7YoQgFQiYjsWdNl-gNAEImPoV" xr:uid="{4ABF3ED5-35CC-480C-A453-63B752374AEE}"/>
+    <hyperlink ref="D2" r:id="rId2" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL" xr:uid="{34F927FB-8968-470B-B62E-18B22CA7017A}"/>
+    <hyperlink ref="D3" r:id="rId3" location="G1oAa6kFLvZNQG8Zt8Qe23rxLx0LNsim0B" xr:uid="{EE09EE68-E8FD-4093-A9EC-9D5CABFBCAA2}"/>
+    <hyperlink ref="D4" r:id="rId4" location="G1cn6NAIUYOxWUz6hHUKNy_y4dG_9MVk_E" display="InventoriesService" xr:uid="{735F4090-F430-413E-822E-D0896CD66F30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sequence for stock service #1
Signed-off-by: chavp <my.parinya@gmail.com>
</commit_message>
<xml_diff>
--- a/DetailsSpec/Stock_details_spec.xlsx
+++ b/DetailsSpec/Stock_details_spec.xlsx
@@ -1,13 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594FF688-D52A-4A37-9D03-3154227A1045}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stock Service" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapping Model -&gt; DTO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="99">
   <si>
     <t>#</t>
   </si>
@@ -142,13 +144,187 @@
   </si>
   <si>
     <t>Sahapat.Orders.Repositories</t>
+  </si>
+  <si>
+    <t>BillTDTO</t>
+  </si>
+  <si>
+    <t>BillTNumber</t>
+  </si>
+  <si>
+    <t>ShipmentType</t>
+  </si>
+  <si>
+    <t>BookNumber</t>
+  </si>
+  <si>
+    <t>ShipmentStatus</t>
+  </si>
+  <si>
+    <t>ShipmentStatusDate</t>
+  </si>
+  <si>
+    <t>FromStockCode</t>
+  </si>
+  <si>
+    <t>ToStockCode</t>
+  </si>
+  <si>
+    <t>ToStockAddress</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>ShipmentStatusType</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>{Scheduled, Shipped, Received, Cancled}</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>StatusDate</t>
+  </si>
+  <si>
+    <t>StockCode</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>ContactPostalAddress</t>
+  </si>
+  <si>
+    <t>PostalAddressDTO</t>
+  </si>
+  <si>
+    <t>HouseNo</t>
+  </si>
+  <si>
+    <t>Street</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Khet</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Tumbon</t>
+  </si>
+  <si>
+    <t>Aumper</t>
+  </si>
+  <si>
+    <t>PostCode</t>
+  </si>
+  <si>
+    <t>ProductDTO</t>
+  </si>
+  <si>
+    <t>ProductCode</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>ProductDescription</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>UnitOfMeasureDesc</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>GoodIdentification</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>OrderItem</t>
+  </si>
+  <si>
+    <t>UnitOfMeasure</t>
+  </si>
+  <si>
+    <t>T-543429</t>
+  </si>
+  <si>
+    <t>Transfer</t>
+  </si>
+  <si>
+    <t>G016</t>
+  </si>
+  <si>
+    <t>R076</t>
+  </si>
+  <si>
+    <t>see PostalAddressDTO</t>
+  </si>
+  <si>
+    <t>เพรชบุรีตัดใหม่</t>
+  </si>
+  <si>
+    <t>บางกะปิ</t>
+  </si>
+  <si>
+    <t>ห้วยขวาง</t>
+  </si>
+  <si>
+    <t>กรุงเทพฯ</t>
+  </si>
+  <si>
+    <t>มองต์เฟลอชนิดมีฟอง300มล.</t>
+  </si>
+  <si>
+    <t>หีบ</t>
+  </si>
+  <si>
+    <t>เรียกดูข้อมูล Stock ของคลังสินค้า</t>
+  </si>
+  <si>
+    <t>#Service_Stock_GetStockByStockCode</t>
+  </si>
+  <si>
+    <t>StockDTO</t>
+  </si>
+  <si>
+    <t>QuantityOnHand</t>
+  </si>
+  <si>
+    <t>บันทีกการรับสินค้าเข้าแล้ว สินค้าจะเพิ่มยอด Stock ให้ทันที</t>
+  </si>
+  <si>
+    <t>#Service_Stock_AdjustedStock</t>
+  </si>
+  <si>
+    <t>เรียกดูข้อมูล BillT ที่ยังไม่รับสินค้าเข้าได้</t>
+  </si>
+  <si>
+    <t>#Service_Stock_GetBillTShipmentNonreceipt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +348,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,8 +368,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -204,12 +404,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -221,6 +439,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -501,26 +738,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.68359375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="48.41796875" customWidth="1"/>
-    <col min="4" max="4" width="50.41796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.578125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -540,7 +777,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -560,7 +797,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
@@ -571,7 +808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>27</v>
       </c>
@@ -582,7 +819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>8</v>
       </c>
@@ -593,7 +830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>16</v>
       </c>
@@ -604,7 +841,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
         <v>17</v>
       </c>
@@ -615,7 +852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>18</v>
       </c>
@@ -626,7 +863,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>19</v>
       </c>
@@ -637,7 +874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>36</v>
       </c>
@@ -648,7 +885,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>6</v>
       </c>
@@ -659,7 +896,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>7</v>
       </c>
@@ -670,7 +907,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>9</v>
       </c>
@@ -681,7 +918,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>10</v>
       </c>
@@ -692,7 +929,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>11</v>
       </c>
@@ -703,7 +940,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>12</v>
       </c>
@@ -714,7 +951,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>2</v>
       </c>
@@ -734,8 +979,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D19" s="1" t="s">
         <v>31</v>
       </c>
       <c r="E19" t="s">
@@ -745,7 +990,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
         <v>33</v>
       </c>
@@ -756,7 +1001,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>32</v>
       </c>
@@ -767,21 +1012,565 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>3</v>
       </c>
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL"/>
-    <hyperlink ref="D3" r:id="rId2" location="G1oAa6kFLvZNQG8Zt8Qe23rxLx0LNsim0B"/>
-    <hyperlink ref="D4" r:id="rId3" location="G1cn6NAIUYOxWUz6hHUKNy_y4dG_9MVk_E" display="InventoriesService"/>
-    <hyperlink ref="C2" r:id="rId4" location="G1GN3B11D7YoQgFQiYjsWdNl-gNAEImPoV" display="#Service_Stock_ListOfOrderFrom21.html"/>
-    <hyperlink ref="C18" r:id="rId5" location="G15_WG0BwxncBmXdwxB0kKU5pd7eugBUKR"/>
-    <hyperlink ref="D18" r:id="rId6" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL"/>
+    <hyperlink ref="D2" r:id="rId1" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" location="G1oAa6kFLvZNQG8Zt8Qe23rxLx0LNsim0B" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" location="G1cn6NAIUYOxWUz6hHUKNy_y4dG_9MVk_E" display="InventoriesService" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" location="G1GN3B11D7YoQgFQiYjsWdNl-gNAEImPoV" display="#Service_Stock_ListOfOrderFrom21.html" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C18" r:id="rId5" location="G15_WG0BwxncBmXdwxB0kKU5pd7eugBUKR" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D18" r:id="rId6" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C23" r:id="rId7" location="G1ev4aFzfxy5qrgjPt6XLO5pu9beFpbJqn" xr:uid="{D21D06A7-D6EB-4F93-88CA-EC451DC80931}"/>
+    <hyperlink ref="D23" r:id="rId8" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL" xr:uid="{741F07CD-0D08-4CF2-993A-EF232BCCF7F2}"/>
+    <hyperlink ref="D24" r:id="rId9" location="G1cn6NAIUYOxWUz6hHUKNy_y4dG_9MVk_E" display="InventoriesService" xr:uid="{F95D2180-103F-490B-97F9-AF186E5FF0E3}"/>
+    <hyperlink ref="D19" r:id="rId10" location="G1YaitPK5Vc72ISfgYvhkJcgWxzW7PnjTG" xr:uid="{87AA7C88-B7D6-448C-8243-C7D81777F719}"/>
+    <hyperlink ref="C27" r:id="rId11" location="G11HwcwaAyD7nboezf7qy303lSkHHkDgMK" xr:uid="{006BEB21-03C5-4F23-8C8C-A1DA1678D105}"/>
+    <hyperlink ref="D27" r:id="rId12" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL" xr:uid="{FC4BB256-1474-434C-AD1D-1D80F2602689}"/>
+    <hyperlink ref="D28" r:id="rId13" location="G1cn6NAIUYOxWUz6hHUKNy_y4dG_9MVk_E" display="InventoriesService" xr:uid="{2A3313BD-6BDB-4117-8F3A-6F9423DDED8E}"/>
+    <hyperlink ref="C30" r:id="rId14" location="G1qLY9t8s66lEy-TBrbC9l2ENSsi_PN1eL" xr:uid="{51400C6D-5D2B-4A5D-B83F-7E1B612D8AE2}"/>
+    <hyperlink ref="D30" r:id="rId15" location="G1J2xWywWx4tBD-WwT4hF07mk5S2uaKEWL" xr:uid="{72A42E23-30E6-4D5E-AA39-EE64978E528F}"/>
+    <hyperlink ref="D31" r:id="rId16" location="G1YaitPK5Vc72ISfgYvhkJcgWxzW7PnjTG" xr:uid="{66A81499-2C5D-4420-955D-1E9B44334556}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9047E1ED-CF17-4DB1-8BCA-90A1B2D87538}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="38.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="12">
+        <v>10310</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="12">
+        <v>785402</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>